<commit_message>
run_IDFs: Fixing Foc, fvalve problems
Trying to fix problems with Foc and fvalve where they are not changing capture from the base-case.
</commit_message>
<xml_diff>
--- a/inputfiles/params_Pine8th.xlsx
+++ b/inputfiles/params_Pine8th.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SubsurfaceSinks\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1259905-C931-40F8-A494-CCD9A728419B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187F65FA-B34D-4C7F-9F5B-A3367CDED3CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="14475" windowHeight="3780" xr2:uid="{DF45CC4F-1F30-4014-8BCA-4F35CD4112BF}"/>
   </bookViews>
@@ -647,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -679,6 +679,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -996,10 +1003,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD8B427-7822-4B11-BEA9-14D81D15628E}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S77"/>
+  <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1721,50 +1728,19 @@
     </row>
     <row r="52" spans="1:19">
       <c r="A52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="3">
-        <v>0.20330967999999999</v>
+        <v>102</v>
+      </c>
+      <c r="B52" s="1">
+        <v>360</v>
       </c>
       <c r="C52" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>174</v>
-      </c>
-      <c r="I52" s="3"/>
+        <v>149</v>
+      </c>
+      <c r="G52" s="3"/>
       <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="A53" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="1">
-        <v>360</v>
-      </c>
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" t="s">
-        <v>149</v>
-      </c>
-      <c r="G53" s="3"/>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:19">
-      <c r="A54" t="s">
-        <v>131</v>
-      </c>
-      <c r="B54" s="11">
-        <v>0.12166552</v>
-      </c>
-      <c r="C54" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" t="s">
-        <v>145</v>
-      </c>
-      <c r="L54" s="2"/>
     </row>
     <row r="55" spans="1:19">
       <c r="A55" t="s">
@@ -2074,8 +2050,8 @@
       <c r="A77" t="s">
         <v>176</v>
       </c>
-      <c r="B77">
-        <v>0.15501755</v>
+      <c r="B77" s="16">
+        <v>0.19768124000000001</v>
       </c>
       <c r="C77" t="s">
         <v>177</v>
@@ -2084,6 +2060,37 @@
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="17">
+        <v>0.11874427999999999</v>
+      </c>
+      <c r="C78" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" t="s">
+        <v>174</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" t="s">
+        <v>131</v>
+      </c>
+      <c r="B79" s="15">
+        <v>0.19605502</v>
+      </c>
+      <c r="C79" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79" t="s">
+        <v>145</v>
+      </c>
+      <c r="L79" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>